<commit_message>
login page code refactoring
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006C60A0-D79A-4488-977D-7842DBB2E078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6075C6-D56D-7E47-A483-639B0F29C835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6800" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +144,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,17 +467,17 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -485,58 +488,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7ED63F57-644F-4E78-9587-08CB51DEF5FB}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{EB480860-584A-43F6-9478-DD4F2553FE6D}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{EB701B42-A320-4932-9568-F231C8F446AB}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{716734F3-6854-43CF-931C-C8D1149FAF15}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FF34B051-1B07-6C46-9722-7B365781AE7E}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{03D9D672-D9AB-1F4C-9CEA-7928D178D0F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>